<commit_message>
commit on oct 10th
</commit_message>
<xml_diff>
--- a/Exceldata/latestorders.xlsx
+++ b/Exceldata/latestorders.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="22">
   <si>
     <t xml:space="preserve">order </t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Steve Gates (steve_gates@nopCommerce.com)</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -144,87 +147,87 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>